<commit_message>
Updated sample sizes accurately for all traits passed to MR
</commit_message>
<xml_diff>
--- a/1_MR/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
+++ b/1_MR/1_data/gwas_summstats/hcm_related_traits_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Chan\Documents\R Projects\Watkins_Offline\MultiPheno_HCM_MR\1_data\gwas_summstats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Chan\Documents\R Projects\Watkins_Offline\MultiPheno_HCM_MR\1_MR\1_data\gwas_summstats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB115851-5682-45B7-873D-7EA4DD888469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B257E73A-D922-4C4C-9236-C0DEA921AB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="3870" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{73FD91AA-0239-4790-95FD-809D24710730}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype Selection" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="234">
   <si>
     <t>TRAIT GROUP</t>
   </si>
@@ -665,9 +665,6 @@
     <t>TnT</t>
   </si>
   <si>
-    <t>POTENTIAL IV</t>
-  </si>
-  <si>
     <t>CAD/Ischemic HD</t>
   </si>
   <si>
@@ -719,10 +716,31 @@
     <t>HF</t>
   </si>
   <si>
-    <t>STKE</t>
-  </si>
-  <si>
     <t>eGFR</t>
+  </si>
+  <si>
+    <t>stroke</t>
+  </si>
+  <si>
+    <t>European (UKB)</t>
+  </si>
+  <si>
+    <t>Heart failure with reduced EF</t>
+  </si>
+  <si>
+    <t>Heart failure with preserved EF</t>
+  </si>
+  <si>
+    <t>HFpEF</t>
+  </si>
+  <si>
+    <t>HFrEF</t>
+  </si>
+  <si>
+    <t>Comorbidities</t>
+  </si>
+  <si>
+    <t>VAR_GROUP</t>
   </si>
 </sst>
 </file>
@@ -857,7 +875,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -920,11 +938,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -932,11 +959,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1321,7 +1354,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1338,7 +1371,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="16" t="s">
         <v>81</v>
       </c>
@@ -1354,16 +1387,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>141</v>
       </c>
       <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>210</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>211</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>137</v>
@@ -1371,16 +1404,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>141</v>
       </c>
       <c r="D6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>210</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>211</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>137</v>
@@ -1388,16 +1421,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>141</v>
       </c>
       <c r="D7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G7" s="16"/>
     </row>
@@ -1416,26 +1449,26 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="33" t="s">
         <v>141</v>
       </c>
       <c r="D10" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="33" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
       <c r="D11" t="s">
         <v>154</v>
       </c>
@@ -1445,10 +1478,10 @@
       <c r="F11" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="33"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="16" t="s">
         <v>150</v>
       </c>
@@ -1456,7 +1489,7 @@
         <v>141</v>
       </c>
       <c r="D12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>167</v>
@@ -1469,7 +1502,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="16" t="s">
         <v>48</v>
       </c>
@@ -1487,7 +1520,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="16" t="s">
         <v>151</v>
       </c>
@@ -1505,7 +1538,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="16" t="s">
         <v>152</v>
       </c>
@@ -1523,61 +1556,61 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
+      <c r="A17" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="33" t="s">
         <v>141</v>
       </c>
       <c r="D17" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="33" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
       <c r="D18" t="s">
         <v>149</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="30"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
       <c r="D19" t="s">
         <v>147</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="30"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
       <c r="D20" t="s">
         <v>148</v>
       </c>
-      <c r="F20" s="32"/>
-      <c r="G20" s="30"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
-      <c r="B21" s="32" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="33" t="s">
         <v>165</v>
       </c>
       <c r="D21" t="s">
@@ -1589,9 +1622,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="30"/>
+      <c r="A22" s="35"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="33"/>
       <c r="D22" t="s">
         <v>175</v>
       </c>
@@ -1604,16 +1637,16 @@
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="34" t="s">
         <v>187</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="33" t="s">
         <v>163</v>
       </c>
       <c r="G24" s="16" t="s">
@@ -1621,62 +1654,68 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
       <c r="G25" s="16" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
       <c r="G26" s="16" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="G27" s="16" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
       <c r="G28" s="16" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
       <c r="G29" s="16" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="G17:G20"/>
     <mergeCell ref="G10:G11"/>
     <mergeCell ref="A3:A4"/>
@@ -1686,12 +1725,6 @@
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="F17:F20"/>
     <mergeCell ref="A10:A15"/>
-    <mergeCell ref="D24:D29"/>
-    <mergeCell ref="C24:C29"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1700,566 +1733,662 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0823BC-1B35-46B4-9DFF-9CD2609C03A7}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="H1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="27" t="s">
+      <c r="I1" s="29"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="I3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="27" t="s">
+      <c r="E3" s="18">
+        <v>74286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="34"/>
+      <c r="B4" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="E4" s="18">
+        <v>1665399</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="I4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="34"/>
       <c r="B5" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" t="s">
         <v>178</v>
       </c>
-      <c r="I5" t="s">
+      <c r="E5" s="18">
+        <v>1328550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E6" s="18">
+        <v>747317</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="34"/>
+      <c r="B7" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" t="s">
+        <v>231</v>
+      </c>
+      <c r="D7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="18">
+        <v>931741</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="34"/>
+      <c r="B8" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>215</v>
+      </c>
+      <c r="E8" s="18">
+        <v>1378170</v>
+      </c>
+      <c r="G8" t="s">
+        <v>222</v>
+      </c>
+      <c r="H8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="18">
+        <f>23991+264655+1308460+5662+11312</f>
+        <v>1614080</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="H9" t="s">
+        <v>219</v>
+      </c>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="18">
+        <v>719432</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1028980</v>
+      </c>
+      <c r="F12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="18">
+        <f>177415+490089</f>
+        <v>667504</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="34"/>
+      <c r="B14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="18">
+        <v>632802</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="C6" t="s">
-        <v>216</v>
-      </c>
-      <c r="F6" t="s">
-        <v>223</v>
-      </c>
-      <c r="G6" t="s">
-        <v>217</v>
-      </c>
-      <c r="I6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" t="s">
-        <v>221</v>
-      </c>
-      <c r="F7" t="s">
-        <v>222</v>
-      </c>
-      <c r="G7" t="s">
-        <v>220</v>
-      </c>
-      <c r="I7" t="s">
-        <v>226</v>
-      </c>
-      <c r="M7" s="16"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
-        <v>218</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D15" t="s">
         <v>113</v>
       </c>
-      <c r="I8" t="s">
+      <c r="E15" s="18">
+        <v>406504</v>
+      </c>
+      <c r="F15" t="s">
         <v>227</v>
       </c>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="1">
-        <v>650000</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1028980</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="1">
-        <f>490089+177415</f>
-        <v>667504</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1232091</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-    </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B17" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D17" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E17" s="18">
         <v>43881</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F17" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="G17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H17" t="s">
         <v>27</v>
       </c>
-      <c r="I15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
-      <c r="B16" s="27" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D18" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
+      <c r="E18" s="18">
+        <v>2374</v>
+      </c>
+      <c r="F18" t="s">
         <v>190</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="I16" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="27" t="s">
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="34"/>
+      <c r="B19" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C19" t="s">
+        <v>200</v>
+      </c>
+      <c r="D19" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
+      <c r="E19" s="18">
+        <v>2374</v>
+      </c>
+      <c r="F19" t="s">
         <v>190</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="I17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="27" t="s">
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C20" t="s">
+        <v>201</v>
+      </c>
+      <c r="D20" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E20" s="18">
         <v>39561</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G20" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H20" t="s">
         <v>63</v>
       </c>
-      <c r="I18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
-      <c r="B19" s="27" t="s">
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="34"/>
+      <c r="B21" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E21" s="18">
         <v>39559</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F21" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G21" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H21" t="s">
         <v>63</v>
       </c>
-      <c r="I19" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
-      <c r="B20" s="27" t="s">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="34"/>
+      <c r="B22" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E22" s="18">
         <v>39560</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F22" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="G22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H22" t="s">
         <v>63</v>
       </c>
-      <c r="I20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B24" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="18">
+        <v>48128</v>
+      </c>
+      <c r="F24" t="s">
         <v>26</v>
       </c>
-      <c r="I22" t="s">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="34"/>
+      <c r="B25" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C25" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="18">
+        <v>48128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" t="s">
+        <v>204</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="18">
+        <v>48128</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="34"/>
+      <c r="B27" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="37"/>
+      <c r="E27" s="18">
+        <v>48128</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="34"/>
+      <c r="B28" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="18">
+        <v>48128</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="34"/>
+      <c r="B29" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D29" s="37"/>
+      <c r="E29" s="18">
+        <v>48128</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="D30" s="32"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B31" s="16" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="E23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="C24" s="32"/>
-      <c r="E24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" s="16" t="s">
+      <c r="C31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E31" s="18">
+        <v>2465</v>
+      </c>
+      <c r="F31" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="34"/>
+      <c r="B32" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" t="s">
+        <v>207</v>
+      </c>
+      <c r="D32" s="38"/>
+      <c r="E32" s="18">
+        <v>2465</v>
+      </c>
+      <c r="F32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="34"/>
+      <c r="B33" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="E25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="C33" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="B26" s="16" t="s">
+      <c r="D33" s="38"/>
+      <c r="E33" s="18">
+        <v>2465</v>
+      </c>
+      <c r="F33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="34"/>
+      <c r="B34" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="E26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="C34" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" s="16" t="s">
+      <c r="D34" s="38"/>
+      <c r="E34" s="18">
+        <v>2465</v>
+      </c>
+      <c r="F34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="34"/>
+      <c r="B35" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="E27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="C35" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D35" s="38"/>
+      <c r="E35" s="18">
+        <v>2465</v>
+      </c>
+      <c r="F35" t="s">
         <v>190</v>
       </c>
-      <c r="I29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="E30" s="1" t="s">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="34"/>
+      <c r="B36" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="38"/>
+      <c r="E36" s="18">
+        <v>2465</v>
+      </c>
+      <c r="F36" t="s">
         <v>190</v>
       </c>
-      <c r="I30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C31" s="32"/>
-      <c r="E31" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C32" s="32"/>
-      <c r="E32" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I32" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C33" s="32"/>
-      <c r="E33" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="E34" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I34" t="s">
-        <v>191</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A22:A27"/>
+  <mergeCells count="7">
+    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="D24:D29"/>
+    <mergeCell ref="D31:D36"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="A31:A36"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F10" r:id="rId1" xr:uid="{B83954B4-B6D1-48BF-9B2E-8905E8FFD0A7}"/>
-    <hyperlink ref="G10" r:id="rId2" xr:uid="{957338A5-BC66-49D5-8609-3080023068F3}"/>
-    <hyperlink ref="F12" r:id="rId3" xr:uid="{138926C0-AD4A-4096-9A20-9E03FD133BF5}"/>
-    <hyperlink ref="G12" r:id="rId4" xr:uid="{0E297714-3FE4-4E9F-9F33-B16DA1AFEADA}"/>
-    <hyperlink ref="F13" r:id="rId5" xr:uid="{ABE989B2-0C0E-49D2-AF4B-165CA780079F}"/>
-    <hyperlink ref="G13" r:id="rId6" xr:uid="{60EBE0DE-158D-42FA-AA25-7D402307C060}"/>
-    <hyperlink ref="G11" r:id="rId7" xr:uid="{E8A5F076-70E4-4277-8F21-61AFC17F73FE}"/>
-    <hyperlink ref="F15" r:id="rId8" xr:uid="{EEB667E5-44BE-44E4-B491-53F3A8E8504F}"/>
-    <hyperlink ref="F19" r:id="rId9" xr:uid="{28212A0C-B9FD-46E8-B44E-D8ACF717F21F}"/>
-    <hyperlink ref="F20" r:id="rId10" xr:uid="{97167BEB-91A0-4AAE-A67E-6AF177E3CDC0}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{5BC3D297-B9F4-4C2E-AF0F-00B940C4F351}"/>
+    <hyperlink ref="G11" r:id="rId1" xr:uid="{B83954B4-B6D1-48BF-9B2E-8905E8FFD0A7}"/>
+    <hyperlink ref="H11" r:id="rId2" xr:uid="{957338A5-BC66-49D5-8609-3080023068F3}"/>
+    <hyperlink ref="G13" r:id="rId3" xr:uid="{138926C0-AD4A-4096-9A20-9E03FD133BF5}"/>
+    <hyperlink ref="H13" r:id="rId4" xr:uid="{0E297714-3FE4-4E9F-9F33-B16DA1AFEADA}"/>
+    <hyperlink ref="G14" r:id="rId5" xr:uid="{ABE989B2-0C0E-49D2-AF4B-165CA780079F}"/>
+    <hyperlink ref="H14" r:id="rId6" xr:uid="{60EBE0DE-158D-42FA-AA25-7D402307C060}"/>
+    <hyperlink ref="H12" r:id="rId7" xr:uid="{E8A5F076-70E4-4277-8F21-61AFC17F73FE}"/>
+    <hyperlink ref="G17" r:id="rId8" xr:uid="{EEB667E5-44BE-44E4-B491-53F3A8E8504F}"/>
+    <hyperlink ref="G21" r:id="rId9" xr:uid="{28212A0C-B9FD-46E8-B44E-D8ACF717F21F}"/>
+    <hyperlink ref="G22" r:id="rId10" xr:uid="{97167BEB-91A0-4AAE-A67E-6AF177E3CDC0}"/>
+    <hyperlink ref="G20" r:id="rId11" xr:uid="{5BC3D297-B9F4-4C2E-AF0F-00B940C4F351}"/>
+    <hyperlink ref="G9" r:id="rId12" xr:uid="{7ACBABCD-1757-472B-9D5D-0F56C5F00B3A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3114,14 +3243,14 @@
       <c r="B1" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="F1" s="34" t="s">
+      <c r="D1" s="39"/>
+      <c r="F1" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" s="20" t="s">
@@ -3138,7 +3267,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -3158,7 +3287,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
+      <c r="A4" s="34"/>
       <c r="B4" s="21" t="s">
         <v>59</v>
       </c>
@@ -3167,7 +3296,7 @@
       <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="34" t="s">
         <v>129</v>
       </c>
       <c r="B6" s="21" t="s">
@@ -3181,7 +3310,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="21" t="s">
         <v>106</v>
       </c>
@@ -3193,7 +3322,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="21" t="s">
         <v>48</v>
       </c>
@@ -3205,7 +3334,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="21" t="s">
         <v>52</v>
       </c>
@@ -3217,7 +3346,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="21" t="s">
         <v>57</v>
       </c>
@@ -3229,7 +3358,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="34" t="s">
         <v>131</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -3237,31 +3366,31 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="21" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="35" t="s">
         <v>132</v>
       </c>
       <c r="B18" s="21" t="s">
@@ -3275,7 +3404,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="21" t="s">
         <v>68</v>
       </c>
@@ -3287,7 +3416,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="21" t="s">
         <v>69</v>
       </c>
@@ -3299,7 +3428,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="21" t="s">
         <v>70</v>
       </c>

</xml_diff>